<commit_message>
minor revision to scenarios paths distribution and minor bug correction
</commit_message>
<xml_diff>
--- a/arpascm/ARPA_logistics_metrics_v2.0_Scenario_1_non_critico.xlsx
+++ b/arpascm/ARPA_logistics_metrics_v2.0_Scenario_1_non_critico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.pinto\PycharmProjects\ARPA-FCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4971ED-9524-4E23-8050-8CFAB179B484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F45A58-35D2-4BF3-96F2-CB42359BEC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -568,13 +568,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
@@ -1507,10 +1507,10 @@
         <v>29</v>
       </c>
       <c r="F12" s="2">
-        <v>45024.70821759259</v>
+        <v>44659.70821759259</v>
       </c>
       <c r="G12" s="2">
-        <v>45028.481203703697</v>
+        <v>44663.481203703705</v>
       </c>
       <c r="H12">
         <v>2</v>

</xml_diff>